<commit_message>
Added new output data
</commit_message>
<xml_diff>
--- a/Data Analysis for Group Technical Report.xlsx
+++ b/Data Analysis for Group Technical Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10711"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura\Documents\Classes\ISE 2004\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Macbook Pro/Georgia Tech/Fall 2020/ISYE 3132 - Stochastic Manufacturing Proceses/Optimization-of-Inventory-Policy-DTMC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88CE1339-E73E-4975-92D9-88C1F5364EAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E69D6F-7710-B940-B9BE-373FBB338559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="17820" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results Summary" sheetId="12" r:id="rId1"/>
@@ -472,21 +472,21 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="41" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="40.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -501,7 +501,7 @@
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -536,7 +536,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -571,7 +571,7 @@
         <v>481.51187565240497</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -606,7 +606,7 @@
         <v>485.87823366505143</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -641,7 +641,7 @@
         <v>450.04671467347606</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -676,7 +676,7 @@
         <v>477.69017655678937</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -711,7 +711,7 @@
         <v>430.85718879214096</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -746,7 +746,7 @@
         <v>417.86824470111645</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -781,7 +781,7 @@
         <v>416.12342794064494</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -816,7 +816,7 @@
         <v>416.00341718749985</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -851,7 +851,7 @@
         <v>362.97023307627887</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -886,7 +886,7 @@
         <v>373.01817582501087</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -921,7 +921,7 @@
         <v>468.1335580646429</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -956,7 +956,7 @@
         <v>440.85718879214051</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -991,7 +991,7 @@
         <v>427.86824470111583</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>426.12342794064432</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>426.00341718749985</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>238.80853281701422</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>433.26952725059977</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>445.48264456840144</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>437.8682447011152</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>436.12342794064369</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>436.00341718749985</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>443.70612319829507</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>383.79020397956697</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>447.12764514717145</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>446.12342794064313</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>446.00341718749985</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>438.61567127320853</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>455.55060517318498</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>456.07086504163817</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>456.00341718749985</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>388.65391081109067</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>330.24138458240571</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>330.22959156249976</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>60.682484104081283</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>60.695244687500065</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>36</v>
       </c>

</xml_diff>